<commit_message>
Lotta stuff + FII-Anotacoes teste 1 e 2 + IPEIO-slides anotacoes e refat - QF_A-Bibliografia (peter atkins) > fix alias FII,IPEIO,QF_A + QF_A-lab.1 excel
</commit_message>
<xml_diff>
--- a/2022.1-1o_Semestre/QF_A-Quimica_Fisica/QF_A-Laboratórios/QF_A-Lab.1.xlsx
+++ b/2022.1-1o_Semestre/QF_A-Quimica_Fisica/QF_A-Laboratórios/QF_A-Lab.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipepinto/Documents/Assets Cache/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipepinto/Documents/College : Study/FCT - Mestrado Integrado em Engenharia Química e Bioquímica/FCT-MIEQB-Mestrado_Integrado_em_Engenharia_Química_e_Bioquímica/2022.1-1o_Semestre/QF_A-Quimica_Fisica/QF_A-Laboratórios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC5026C1-7931-604F-8EF1-67ECB20D9441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251B64A0-6BED-E74D-87FD-61B115CE46D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4898,7 +4898,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
@@ -6650,7 +6650,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>